<commit_message>
Test-6 for NN (MSE)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-6.xlsx
+++ b/migforecasting/underground/test-6.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>test size 20%</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>С долларом</t>
+  </si>
+  <si>
+    <t>test 20%</t>
+  </si>
+  <si>
+    <t>NN(64,64,64,64,1) (citiesdataset-NY-2.csv) - next year</t>
+  </si>
+  <si>
+    <t>NN(64,64,64,64,1) (citiesdataset-NYDcor-2.csv) - next year</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -131,6 +140,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -195,7 +207,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -300,7 +311,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -421,7 +431,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -564,7 +573,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -676,7 +684,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -716,6 +723,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Обучающая выборка (сред.)</c:v>
+          </c:tx>
           <c:spPr>
             <a:pattFill prst="narHorz">
               <a:fgClr>
@@ -778,7 +788,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -834,6 +843,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Тестовая выборка (сред.)</c:v>
+          </c:tx>
           <c:spPr>
             <a:pattFill prst="narHorz">
               <a:fgClr>
@@ -896,7 +908,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1039,7 +1050,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4721,8 +4731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R65"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7050,10 +7060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T65"/>
+  <dimension ref="C3:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M74" sqref="M74"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7066,9 +7076,13 @@
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="19" max="19" width="12.85546875" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" customWidth="1"/>
+    <col min="30" max="30" width="13" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:31" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7081,8 +7095,14 @@
       <c r="S3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="Y3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -7099,8 +7119,14 @@
         <v>11</v>
       </c>
       <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>2</v>
@@ -7129,8 +7155,20 @@
       <c r="T5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="Y5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -7167,8 +7205,26 @@
       <c r="T6" s="4">
         <v>7.188589138175625E-3</v>
       </c>
-    </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>9.2046183543042614E-4</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>8.3932795195363705E-3</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>7.3633209115142541E-4</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>5.8519338878325836E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f>C6+1</f>
         <v>2</v>
@@ -7209,8 +7265,26 @@
       <c r="T7" s="4">
         <v>7.7804257062983216E-3</v>
       </c>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>4.6212361669082508E-4</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>7.6528724704759774E-3</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>7.9888231501011608E-4</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>6.8831400241856364E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" ref="C8:C55" si="0">C7+1</f>
         <v>3</v>
@@ -7251,8 +7325,26 @@
       <c r="T8" s="4">
         <v>6.6696856910028607E-3</v>
       </c>
-    </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X8" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>7.490812499387127E-4</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>1.124498069401093E-2</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>5.2847515663967891E-4</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>7.7988171750966069E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7293,8 +7385,26 @@
       <c r="T9" s="4">
         <v>5.9363055879915576E-3</v>
       </c>
-    </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X9" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>4.812933503987121E-4</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>6.8430562474151987E-3</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>7.3784660560717271E-4</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>8.3445463924505265E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7335,8 +7445,26 @@
       <c r="T10" s="4">
         <v>5.3224483331998909E-3</v>
       </c>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X10" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>6.8160087661717043E-4</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>6.8568495864527396E-3</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>6.7566018680901348E-4</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>6.7695682726361759E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7377,8 +7505,26 @@
       <c r="T11" s="4">
         <v>6.2013696772142551E-3</v>
       </c>
-    </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X11" s="2">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>1.014814980638644E-3</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>1.117754553937866E-2</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>7.4603137664475204E-4</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>5.2908399675477436E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7419,8 +7565,26 @@
       <c r="T12" s="4">
         <v>5.6543061741757593E-3</v>
       </c>
-    </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X12" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>1.2268214597950171E-3</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>7.4675544438988503E-3</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>8.5461614420526068E-4</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>7.5723420678569789E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7461,8 +7625,26 @@
       <c r="T13" s="4">
         <v>5.2400764157673483E-3</v>
       </c>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X13" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>3.4457929102472891E-4</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>6.6591300353251578E-3</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>8</v>
+      </c>
+      <c r="AD13" s="4">
+        <v>8.0225781711322768E-4</v>
+      </c>
+      <c r="AE13" s="4">
+        <v>6.5701747767989028E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7503,8 +7685,26 @@
       <c r="T14" s="4">
         <v>6.171111497584196E-3</v>
       </c>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X14" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>6.1613838624861134E-4</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>8.8318782515261658E-3</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD14" s="4">
+        <v>6.030543654711412E-4</v>
+      </c>
+      <c r="AE14" s="4">
+        <v>6.4142820345973548E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7545,8 +7745,26 @@
       <c r="T15" s="4">
         <v>7.4878625358643144E-3</v>
       </c>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X15" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>2.8212759633885408E-4</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>1.256871074707251E-2</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>10</v>
+      </c>
+      <c r="AD15" s="4">
+        <v>5.6667908344708545E-4</v>
+      </c>
+      <c r="AE15" s="4">
+        <v>3.9588352293645664E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7587,8 +7805,26 @@
       <c r="T16" s="4">
         <v>6.3463839251047677E-3</v>
       </c>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X16" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>3.8192327472772489E-4</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>7.2203541455874024E-3</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>11</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>6.6231979516758984E-4</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>4.8058731150736039E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7629,8 +7865,26 @@
       <c r="T17" s="4">
         <v>6.0561760994672104E-3</v>
       </c>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X17" s="2">
+        <v>12</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>9.771344439018679E-4</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>7.9873452337947438E-3</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>12</v>
+      </c>
+      <c r="AD17" s="4">
+        <v>1.3394902435832491E-3</v>
+      </c>
+      <c r="AE17" s="4">
+        <v>6.73090900852737E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7671,8 +7925,26 @@
       <c r="T18" s="4">
         <v>8.9994365285987581E-3</v>
       </c>
-    </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X18" s="2">
+        <v>13</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>2.6288827336013411E-3</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>7.0475122901448211E-3</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>13</v>
+      </c>
+      <c r="AD18" s="4">
+        <v>7.9983205533728911E-4</v>
+      </c>
+      <c r="AE18" s="4">
+        <v>5.3456310515376474E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7713,8 +7985,26 @@
       <c r="T19" s="4">
         <v>6.2915048880807451E-3</v>
       </c>
-    </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X19" s="2">
+        <v>14</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>5.4026527000035189E-4</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>7.5757849929986828E-3</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>14</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>6.097937522010757E-4</v>
+      </c>
+      <c r="AE19" s="4">
+        <v>7.2697126605409659E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7755,8 +8045,26 @@
       <c r="T20" s="4">
         <v>7.6209223236169401E-3</v>
       </c>
-    </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X20" s="2">
+        <v>15</v>
+      </c>
+      <c r="Y20" s="4">
+        <v>4.8317013864743533E-4</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>1.0876356917816941E-2</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>15</v>
+      </c>
+      <c r="AD20" s="4">
+        <v>7.7297783224082042E-4</v>
+      </c>
+      <c r="AE20" s="4">
+        <v>4.8582432484114242E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7797,8 +8105,26 @@
       <c r="T21" s="4">
         <v>5.2901226478457297E-3</v>
       </c>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X21" s="2">
+        <v>16</v>
+      </c>
+      <c r="Y21" s="4">
+        <v>4.0908375660599658E-4</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>9.4463593439375656E-3</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>16</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>4.7186448306659558E-4</v>
+      </c>
+      <c r="AE21" s="4">
+        <v>5.6754989077258721E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7839,8 +8165,26 @@
       <c r="T22" s="4">
         <v>7.5334594583586524E-3</v>
       </c>
-    </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X22" s="2">
+        <v>17</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>3.0686784465563049E-4</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>8.3865697230411877E-3</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>17</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>5.4953746718818571E-4</v>
+      </c>
+      <c r="AE22" s="4">
+        <v>6.1779256644736878E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7881,8 +8225,26 @@
       <c r="T23" s="4">
         <v>8.506565276954637E-3</v>
       </c>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X23" s="2">
+        <v>18</v>
+      </c>
+      <c r="Y23" s="4">
+        <v>1.420066395684231E-3</v>
+      </c>
+      <c r="Z23" s="4">
+        <v>7.7057705457456611E-3</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>18</v>
+      </c>
+      <c r="AD23" s="4">
+        <v>5.7602052353656035E-4</v>
+      </c>
+      <c r="AE23" s="4">
+        <v>6.4564795371807437E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7923,8 +8285,26 @@
       <c r="T24" s="4">
         <v>6.0298183763753312E-3</v>
       </c>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X24" s="2">
+        <v>19</v>
+      </c>
+      <c r="Y24" s="4">
+        <v>3.4848228971280963E-4</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>8.3972866565599196E-3</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD24" s="4">
+        <v>4.4829516185451181E-4</v>
+      </c>
+      <c r="AE24" s="4">
+        <v>6.4220702589115842E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7965,8 +8345,26 @@
       <c r="T25" s="4">
         <v>5.0803260495208332E-3</v>
       </c>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X25" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y25" s="4">
+        <v>5.6687513752917327E-4</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>5.651943738905452E-3</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD25" s="4">
+        <v>6.4915634877089857E-4</v>
+      </c>
+      <c r="AE25" s="4">
+        <v>7.3691090975262627E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8007,8 +8405,14 @@
       <c r="T26" s="4">
         <v>5.5998643233791251E-3</v>
       </c>
-    </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X26" s="2"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="5"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="5"/>
+    </row>
+    <row r="27" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8049,8 +8453,30 @@
       <c r="T27" s="4">
         <v>8.2932104694559815E-3</v>
       </c>
-    </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="4">
+        <f>AVERAGE(Y6:Y25)</f>
+        <v>7.4208969640941324E-4</v>
+      </c>
+      <c r="Z27" s="4">
+        <f>AVERAGE(Z6:Z25)</f>
+        <v>8.3995570561812474E-3</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="4">
+        <f>AVERAGE(AD6:AD25)</f>
+        <v>6.9645614025228236E-4</v>
+      </c>
+      <c r="AE27" s="4">
+        <f>AVERAGE(AE6:AE25)</f>
+        <v>6.3282966189138114E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -8091,8 +8517,30 @@
       <c r="T28" s="4">
         <v>6.1029082484710092E-3</v>
       </c>
-    </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="4">
+        <f>_xlfn.STDEV.S(Y6:Y25)</f>
+        <v>5.4652125350068378E-4</v>
+      </c>
+      <c r="Z28" s="4">
+        <f>_xlfn.STDEV.S(Z6:Z25)</f>
+        <v>1.8059641235904174E-3</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD28" s="4">
+        <f>_xlfn.STDEV.S(AD6:AD25)</f>
+        <v>1.9135799773252029E-4</v>
+      </c>
+      <c r="AE28" s="4">
+        <f>_xlfn.STDEV.S(AE6:AE25)</f>
+        <v>1.1076645031534308E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8134,7 +8582,7 @@
         <v>8.4186838127129366E-3</v>
       </c>
     </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8176,7 +8624,7 @@
         <v>5.786722620280035E-3</v>
       </c>
     </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8218,7 +8666,7 @@
         <v>6.1600098031003641E-3</v>
       </c>
     </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>27</v>

</xml_diff>

<commit_message>
Test-7 NN (nextyear, MSE)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-6.xlsx
+++ b/migforecasting/underground/test-6.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
   <si>
     <t>test size 20%</t>
   </si>
@@ -207,6 +207,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -311,6 +312,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -431,6 +433,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -573,6 +576,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -684,6 +688,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -788,6 +793,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -908,6 +914,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1050,6 +1057,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2094,6 +2102,489 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>Прогноз следующего</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" baseline="0"/>
+              <a:t> года </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>NN)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$Z$63:$AA$63</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без доллара</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С долларом</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$Z$64:$AA$64</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.4208969640941324E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9645614025228236E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEB2-48CF-9F9F-388DA47BD2D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$Z$63:$AA$63</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без доллара</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С долларом</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$Z$65:$AA$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.3995570561812474E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3282966189138114E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEB2-48CF-9F9F-388DA47BD2D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="976238063"/>
+        <c:axId val="976236815"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="976238063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="976236815"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="976236815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="976238063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2254,6 +2745,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
@@ -3812,6 +4343,525 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4458,6 +5508,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4731,7 +5813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R65"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
@@ -7062,8 +8144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView tabSelected="1" topLeftCell="L52" workbookViewId="0">
+      <selection activeCell="AD60" sqref="AD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9380,7 +10462,7 @@
         <v>7.3723734744607361E-3</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9422,7 +10504,7 @@
         <v>8.3334529929859191E-3</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9464,7 +10546,7 @@
         <v>8.5423827329833488E-3</v>
       </c>
     </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9506,7 +10588,7 @@
         <v>8.553913185071366E-3</v>
       </c>
     </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9548,7 +10630,7 @@
         <v>6.0856000631264243E-3</v>
       </c>
     </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9590,7 +10672,7 @@
         <v>6.5573749879574636E-3</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9632,7 +10714,7 @@
         <v>6.8350337523916133E-3</v>
       </c>
     </row>
-    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C55" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9674,7 +10756,7 @@
         <v>7.7414058846469657E-3</v>
       </c>
     </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -9720,7 +10802,7 @@
         <v>6.6916805518296551E-3</v>
       </c>
     </row>
-    <row r="58" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>5</v>
       </c>
@@ -9766,7 +10848,7 @@
         <v>1.157187663638646E-3</v>
       </c>
     </row>
-    <row r="63" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:27" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
         <v>14</v>
       </c>
@@ -9779,8 +10861,14 @@
       <c r="P63" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="Z63" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>12</v>
       </c>
@@ -9799,8 +10887,17 @@
       <c r="P64" s="4">
         <v>9.2949821647087471E-4</v>
       </c>
-    </row>
-    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="Y64" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z64" s="4">
+        <v>7.4208969640941324E-4</v>
+      </c>
+      <c r="AA64" s="4">
+        <v>6.9645614025228236E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>13</v>
       </c>
@@ -9818,6 +10915,15 @@
       </c>
       <c r="P65" s="4">
         <v>6.6916805518296551E-3</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z65" s="4">
+        <v>8.3995570561812474E-3</v>
+      </c>
+      <c r="AA65" s="4">
+        <v>6.3282966189138114E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>